<commit_message>
made changes to tasking
</commit_message>
<xml_diff>
--- a/assignment9/Assignment 9 Sprint 1 Backlog.xlsx
+++ b/assignment9/Assignment 9 Sprint 1 Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Very High</t>
   </si>
@@ -46,9 +46,6 @@
 Mark: Product Owner
 Aaron: Scrub Master
 Sam: Team Member</t>
-  </si>
-  <si>
-    <t>AE</t>
   </si>
   <si>
     <t>Team</t>
@@ -112,15 +109,6 @@
     <t>Research on UML diagrams</t>
   </si>
   <si>
-    <t>Research how to interface to BeetleDev.com webService to calculate BMI</t>
-  </si>
-  <si>
-    <t>Research how to interface to Google API webService</t>
-  </si>
-  <si>
-    <t>Look at how to utilize code from BeetleDev.com (Also in a jar file on Blackboard</t>
-  </si>
-  <si>
     <t>Determine what UML diagrams to use</t>
   </si>
   <si>
@@ -151,9 +139,6 @@
     <t>Sam</t>
   </si>
   <si>
-    <t>Define User Stories</t>
-  </si>
-  <si>
     <t>Create Product Backlog</t>
   </si>
   <si>
@@ -169,10 +154,67 @@
     <t>Check Style</t>
   </si>
   <si>
-    <t>Ad-Hoc (Misc) testing</t>
-  </si>
-  <si>
-    <t>Error corrections/bug fixes</t>
+    <t>Research how to interface UI to Google API webService</t>
+  </si>
+  <si>
+    <t>Research how to output summary data to Google Charts</t>
+  </si>
+  <si>
+    <t>Human centered design and layout of UI</t>
+  </si>
+  <si>
+    <t>Research how to interface UI to BeetleDev.com webService to calculate BMI</t>
+  </si>
+  <si>
+    <t>Look into how to code and output user input for BMI to BeetleDev.com webService to calculate BMI</t>
+  </si>
+  <si>
+    <t>Decide which classes and functions to utilize from BeetleDev.com for BMI</t>
+  </si>
+  <si>
+    <t>Look at and understand how to utilize code from BeetleDev.com (Also in a jar file on Blackboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design UML diagrams in MS Viso </t>
+  </si>
+  <si>
+    <t>Modifications to diagrams in MS Viso</t>
+  </si>
+  <si>
+    <t>Integrate Google API web service</t>
+  </si>
+  <si>
+    <t>Integrate BeetleDev web service</t>
+  </si>
+  <si>
+    <t>Ad-Hoc (Misc) testing  for BMI calculations</t>
+  </si>
+  <si>
+    <t>Ad-Hoc (Misc) testing summary data output</t>
+  </si>
+  <si>
+    <t>Ad-Hoc (Misc) testing for UI and client output data</t>
+  </si>
+  <si>
+    <t>Ad-Hoc (Misc) testing  for Google API chart output</t>
+  </si>
+  <si>
+    <t>Error corrections/bug fixes- summary data output</t>
+  </si>
+  <si>
+    <t>Error corrections/bug fixes- for BMI calculations</t>
+  </si>
+  <si>
+    <t>Error corrections/bug fixes- for UI and client output data</t>
+  </si>
+  <si>
+    <t>Error corrections/bug fixes-  for Google API chart output</t>
+  </si>
+  <si>
+    <t>Aaron/Sam</t>
+  </si>
+  <si>
+    <t>…..</t>
   </si>
 </sst>
 </file>
@@ -413,7 +455,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -593,11 +634,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="940391232"/>
-        <c:axId val="940396128"/>
+        <c:axId val="-979859104"/>
+        <c:axId val="-979867264"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="940391232"/>
+        <c:axId val="-979859104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42695"/>
@@ -642,14 +683,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940396128"/>
+        <c:crossAx val="-979867264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="940396128"/>
+        <c:axId val="-979867264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="104"/>
@@ -702,7 +743,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940391232"/>
+        <c:crossAx val="-979859104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -969,11 +1010,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="940398848"/>
-        <c:axId val="940395040"/>
+        <c:axId val="-979867808"/>
+        <c:axId val="-979866720"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="940398848"/>
+        <c:axId val="-979867808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42695"/>
@@ -1021,7 +1062,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1088,14 +1128,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940395040"/>
+        <c:crossAx val="-979866720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="940395040"/>
+        <c:axId val="-979866720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="104"/>
@@ -1148,7 +1188,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1215,7 +1254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940398848"/>
+        <c:crossAx val="-979867808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2720,10 +2759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2751,7 +2790,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>4</v>
@@ -2771,14 +2810,14 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="9">
         <v>0.5</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
@@ -2792,112 +2831,112 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="9">
         <v>0.1</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D11" s="9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="9">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="21" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D13" s="9">
         <v>2</v>
@@ -2910,99 +2949,98 @@
     <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="21" t="s">
-        <v>30</v>
+      <c r="C14" s="25" t="s">
+        <v>16</v>
       </c>
       <c r="D14" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="25" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D15" s="9">
         <v>1</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="25" t="s">
-        <v>17</v>
+      <c r="C16" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D16" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="26" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D17" s="9">
         <v>2</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="26" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D18" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="26" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D19" s="9">
         <v>1</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="13"/>
+      <c r="C20" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="14">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
@@ -3015,78 +3053,78 @@
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="13"/>
       <c r="C22" s="25" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D22" s="14">
         <v>1</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="13"/>
       <c r="C23" s="25" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D23" s="14">
         <v>1</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="13"/>
       <c r="C24" s="25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D24" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="13"/>
       <c r="C25" s="25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D25" s="14">
         <v>2</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="9" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B26" s="13"/>
       <c r="C26" s="25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D26" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="9" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B27" s="13"/>
       <c r="C27" s="25" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D27" s="14">
         <v>4</v>
@@ -3099,57 +3137,56 @@
     <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B28" s="13"/>
       <c r="C28" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28" s="14">
         <v>4</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B29" s="13"/>
       <c r="C29" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="14">
+        <v>53</v>
+      </c>
+      <c r="D29" s="13">
         <v>4</v>
       </c>
-      <c r="E29" s="14"/>
       <c r="F29" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="13"/>
-      <c r="C30" s="25" t="s">
-        <v>36</v>
+      <c r="C30" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="D30" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" s="13"/>
       <c r="C31" s="22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D31" s="13">
         <v>2</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" s="13"/>
       <c r="C32" s="22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D32" s="13">
         <v>2</v>
@@ -3161,122 +3198,117 @@
     <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="13"/>
       <c r="C33" s="22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D33" s="13">
         <v>2</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="13"/>
       <c r="C34" s="22" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D34" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="13"/>
       <c r="C35" s="22" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D35" s="13">
         <v>4</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="13"/>
       <c r="C36" s="22" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D36" s="13">
         <v>4</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" s="13"/>
       <c r="C37" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="13">
+        <v>57</v>
+      </c>
+      <c r="D37" s="14">
         <v>4</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="13"/>
       <c r="C38" s="22" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D38" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="13"/>
       <c r="C39" s="22" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D39" s="14">
         <v>2</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="13"/>
       <c r="C40" s="22" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D40" s="14">
         <v>2</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41" s="13"/>
       <c r="C41" s="22" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D41" s="14">
         <v>2</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="13"/>
       <c r="C42" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="14">
-        <v>2</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>41</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="13"/>
@@ -3285,22 +3317,20 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B44" s="13"/>
-      <c r="C44" s="22"/>
+      <c r="C44" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="13">
+        <f>SUM(D4:D41)</f>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="E44" s="13">
+        <f>SUM(E4:E29)</f>
+        <v>0</v>
+      </c>
       <c r="F44" s="13"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B45" s="13"/>
-      <c r="C45" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="13">
-        <f>SUM(D4:D42)</f>
-        <v>76.099999999999994</v>
-      </c>
-      <c r="E45" s="13">
-        <f>SUM(E4:E30)</f>
-        <v>0</v>
-      </c>
       <c r="F45" s="13"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.35">
@@ -3320,9 +3350,6 @@
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F52" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3348,13 +3375,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -3421,7 +3448,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="18"/>
     </row>
@@ -3441,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="18"/>
     </row>
@@ -3461,7 +3488,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="18"/>
     </row>
@@ -3474,7 +3501,7 @@
         <v>7.5</v>
       </c>
       <c r="C8" s="9">
-        <f>'Sprint 1'!D13</f>
+        <f>'Sprint 1'!D12</f>
         <v>2</v>
       </c>
       <c r="D8" s="9">
@@ -3494,14 +3521,14 @@
         <v>6.5</v>
       </c>
       <c r="C9" s="9">
-        <f>'Sprint 1'!D15</f>
+        <f>'Sprint 1'!D14</f>
         <v>1</v>
       </c>
       <c r="D9" s="9">
         <v>7</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="18"/>
     </row>
@@ -3514,14 +3541,14 @@
         <v>5.5</v>
       </c>
       <c r="C10" s="9">
-        <f>'Sprint 1'!D16</f>
+        <f>'Sprint 1'!D15</f>
         <v>1</v>
       </c>
       <c r="D10" s="9">
         <v>8</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="18"/>
     </row>
@@ -3534,14 +3561,14 @@
         <v>3.5</v>
       </c>
       <c r="C11" s="9">
-        <f>'Sprint 1'!D17</f>
+        <f>'Sprint 1'!D16</f>
         <v>2</v>
       </c>
       <c r="D11" s="9">
         <v>9</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="18"/>
     </row>
@@ -3561,7 +3588,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="18"/>
     </row>
@@ -3574,14 +3601,14 @@
         <v>#REF!</v>
       </c>
       <c r="C13" s="9">
-        <f>'Sprint 1'!D21</f>
+        <f>'Sprint 1'!D20</f>
         <v>1</v>
       </c>
       <c r="D13" s="13">
         <v>11</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="19"/>
     </row>
@@ -3594,14 +3621,14 @@
         <v>#REF!</v>
       </c>
       <c r="C14" s="9">
-        <f>'Sprint 1'!D23</f>
+        <f>'Sprint 1'!D22</f>
         <v>1</v>
       </c>
       <c r="D14" s="13">
         <v>12</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="19"/>
     </row>
@@ -3614,14 +3641,14 @@
         <v>#REF!</v>
       </c>
       <c r="C15" s="9">
-        <f>'Sprint 1'!D24</f>
+        <f>'Sprint 1'!D23</f>
         <v>1</v>
       </c>
       <c r="D15" s="13">
         <v>13</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="19"/>
     </row>
@@ -3634,14 +3661,14 @@
         <v>#REF!</v>
       </c>
       <c r="C16" s="9">
-        <f>'Sprint 1'!D25</f>
+        <f>'Sprint 1'!D24</f>
         <v>2</v>
       </c>
       <c r="D16" s="13">
         <v>14</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="19"/>
     </row>

</xml_diff>

<commit_message>
Updated actual time - Sam
</commit_message>
<xml_diff>
--- a/assignment9/Assignment 9 Sprint 1 Backlog.xlsx
+++ b/assignment9/Assignment 9 Sprint 1 Backlog.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Chart1" sheetId="3" r:id="rId2"/>
     <sheet name="Burndown Chart" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -220,7 +221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,7 +442,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -623,6 +624,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2C12-49F0-B968-6BB18B52A8DF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -788,7 +794,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1001,6 +1007,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A739-42AD-876C-70D2959FCA37}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2548,6 +2559,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2583,6 +2611,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2761,24 +2806,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1796875" style="1"/>
-    <col min="3" max="3" width="51.1796875" style="13" customWidth="1"/>
-    <col min="4" max="5" width="8.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="51.140625" style="13" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -2796,7 +2841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +2851,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="21" t="s">
@@ -2820,7 +2865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="21" t="s">
@@ -2834,7 +2879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="21" t="s">
@@ -2848,7 +2893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="21" t="s">
@@ -2862,7 +2907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="21" t="s">
@@ -2871,12 +2916,14 @@
       <c r="D8" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9">
+        <v>0.25</v>
+      </c>
       <c r="F8" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="24" t="s">
@@ -2890,7 +2937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="21" t="s">
@@ -2904,7 +2951,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="21" t="s">
@@ -2918,7 +2965,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="21" t="s">
@@ -2932,7 +2979,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="21" t="s">
@@ -2946,7 +2993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="25" t="s">
@@ -2960,7 +3007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="25" t="s">
@@ -2974,7 +3021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="26" t="s">
@@ -2988,7 +3035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="26" t="s">
@@ -3002,7 +3049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="26" t="s">
@@ -3016,7 +3063,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="26" t="s">
@@ -3030,7 +3077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
       <c r="C20" s="25" t="s">
         <v>27</v>
@@ -3043,7 +3090,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="13"/>
       <c r="C21" s="25" t="s">
         <v>28</v>
@@ -3056,7 +3103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
       <c r="C22" s="25" t="s">
         <v>50</v>
@@ -3069,7 +3116,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="C23" s="25" t="s">
         <v>51</v>
@@ -3082,7 +3129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
       <c r="C24" s="25" t="s">
         <v>29</v>
@@ -3095,7 +3142,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="13"/>
       <c r="C25" s="25" t="s">
         <v>30</v>
@@ -3108,7 +3155,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="13"/>
       <c r="C26" s="25" t="s">
         <v>31</v>
@@ -3121,7 +3168,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="13"/>
       <c r="C27" s="25" t="s">
         <v>52</v>
@@ -3134,7 +3181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="13"/>
       <c r="C28" s="25" t="s">
         <v>32</v>
@@ -3147,7 +3194,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="13"/>
       <c r="C29" s="25" t="s">
         <v>53</v>
@@ -3159,7 +3206,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="13"/>
       <c r="C30" s="22" t="s">
         <v>39</v>
@@ -3171,7 +3218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="22" t="s">
         <v>40</v>
@@ -3183,7 +3230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="22" t="s">
         <v>41</v>
@@ -3195,7 +3242,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="13"/>
       <c r="C33" s="22" t="s">
         <v>42</v>
@@ -3207,7 +3254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="13"/>
       <c r="C34" s="22" t="s">
         <v>55</v>
@@ -3219,7 +3266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
       <c r="C35" s="22" t="s">
         <v>54</v>
@@ -3231,7 +3278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="13"/>
       <c r="C36" s="22" t="s">
         <v>56</v>
@@ -3243,7 +3290,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="13"/>
       <c r="C37" s="22" t="s">
         <v>57</v>
@@ -3255,7 +3302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
       <c r="C38" s="22" t="s">
         <v>58</v>
@@ -3267,7 +3314,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="13"/>
       <c r="C39" s="22" t="s">
         <v>59</v>
@@ -3279,7 +3326,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="13"/>
       <c r="C40" s="22" t="s">
         <v>60</v>
@@ -3291,7 +3338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="13"/>
       <c r="C41" s="22" t="s">
         <v>61</v>
@@ -3303,19 +3350,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="13"/>
       <c r="C42" s="22" t="s">
         <v>63</v>
       </c>
       <c r="F42" s="13"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="13"/>
       <c r="C43" s="22"/>
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="13"/>
       <c r="C44" s="13" t="s">
         <v>20</v>
@@ -3326,29 +3373,29 @@
       </c>
       <c r="E44" s="13">
         <f>SUM(E4:E29)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F44" s="13"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F45" s="13"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F46" s="13"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F47" s="13"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F48" s="13"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F49" s="13"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F50" s="13"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F51" s="13"/>
     </row>
   </sheetData>
@@ -3365,15 +3412,15 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3384,7 +3431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>42669</v>
       </c>
@@ -3392,7 +3439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>42669</v>
       </c>
@@ -3412,7 +3459,7 @@
       </c>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>42669</v>
       </c>
@@ -3432,7 +3479,7 @@
       </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>42669</v>
       </c>
@@ -3452,7 +3499,7 @@
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>42670</v>
       </c>
@@ -3472,7 +3519,7 @@
       </c>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>42670</v>
       </c>
@@ -3492,7 +3539,7 @@
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>42670</v>
       </c>
@@ -3512,7 +3559,7 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>42671</v>
       </c>
@@ -3532,7 +3579,7 @@
       </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>42673</v>
       </c>
@@ -3552,7 +3599,7 @@
       </c>
       <c r="F10" s="18"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>42673</v>
       </c>
@@ -3572,7 +3619,7 @@
       </c>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>42673</v>
       </c>
@@ -3592,7 +3639,7 @@
       </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>42674</v>
       </c>
@@ -3612,7 +3659,7 @@
       </c>
       <c r="F13" s="19"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>42675</v>
       </c>
@@ -3632,7 +3679,7 @@
       </c>
       <c r="F14" s="19"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>42675</v>
       </c>
@@ -3652,7 +3699,7 @@
       </c>
       <c r="F15" s="19"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>42675</v>
       </c>

</xml_diff>